<commit_message>
Update package.json with start script
</commit_message>
<xml_diff>
--- a/feedbacks.xlsx
+++ b/feedbacks.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -502,9 +502,169 @@
         <v>2026-02-04T17:43:24.885Z</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>20BEE2001</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Merwin S</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Ok</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="str">
+        <v>2026-02-05T04:52:39.104Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>20BEE2001</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Merwin S</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D7" t="str">
+        <v>excellente</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="str">
+        <v>2026-02-05T04:57:00.418Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>20BEE2001</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Merwin S</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Ok</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="str">
+        <v>2026-02-05T05:03:57.480Z</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>20BEE0001</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Merwin S</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Ok</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="str">
+        <v>2026-02-05T05:11:22.267Z</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>20BEE5984</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Ritwik</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Not bad</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="str">
+        <v>2026-02-05T05:12:03.250Z</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>20BEE2001</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Jershwin S</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Niche</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="str">
+        <v>2026-02-05T05:16:10.354Z</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>20BEE0001</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Merwin S</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="str">
+        <v>2026-02-05T05:18:25.149Z</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>20BEE2001</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Merwin</v>
+      </c>
+      <c r="C13" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Ok</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="str">
+        <v>5/2/2026, 11:12:29 am</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: set server.js as entry point and add start script
</commit_message>
<xml_diff>
--- a/feedbacks.xlsx
+++ b/feedbacks.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -662,9 +662,49 @@
         <v>5/2/2026, 11:12:29 am</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>20BEE2001</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Ram</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Deis Irae</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="str">
+        <v>5/2/2026, 11:25:50 am</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>20BEE2001</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Norman</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Canteen is really clean</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" t="str">
+        <v>5/2/2026, 11:47:10 am</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: bind server to process.env.PORT for Render
</commit_message>
<xml_diff>
--- a/feedbacks.xlsx
+++ b/feedbacks.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -702,9 +702,29 @@
         <v>5/2/2026, 11:47:10 am</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>20BEE2001</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Merwin S</v>
+      </c>
+      <c r="C16" t="str">
+        <v>2020</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Ok</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="str">
+        <v>5/2/2026, 12:00:52 pm</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>